<commit_message>
work through some of updated checklist.
</commit_message>
<xml_diff>
--- a/data/raw/EDA SummaryMarch15_Rizzo.xlsx
+++ b/data/raw/EDA SummaryMarch15_Rizzo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine\Desktop\IT476\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\teradata\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23078AB8-E8C2-4DC7-BE0D-0F33C27B21CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86474099-D334-44EC-A3E1-F21CD1DD1213}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF3F421E-1078-4E2D-8514-4BCF3A33D0AB}"/>
+    <workbookView xWindow="600" yWindow="1485" windowWidth="20520" windowHeight="11475" xr2:uid="{DF3F421E-1078-4E2D-8514-4BCF3A33D0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Type Setting" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="155">
   <si>
     <t>Campaign</t>
   </si>
@@ -901,26 +907,26 @@
   <dimension ref="A1:N110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H106" sqref="H106"/>
+      <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -958,7 +964,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -972,7 +978,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -992,7 +998,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1026,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1057,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1117,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1154,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1171,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1233,7 +1239,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1273,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1391,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1447,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1481,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1498,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1515,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1535,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -1572,7 +1578,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1735,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -1763,7 +1769,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -1780,7 +1786,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -1817,7 +1823,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1834,7 +1840,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1860,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -1894,7 +1900,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -1934,7 +1940,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1978,7 @@
       </c>
       <c r="N60" s="3"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -1989,7 +1995,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -2026,7 +2032,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2046,7 +2052,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -2089,7 +2095,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2138,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2221,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2301,7 +2307,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -2351,7 +2357,7 @@
       </c>
       <c r="N78" s="3"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -2378,7 +2384,7 @@
       </c>
       <c r="N79" s="3"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -2398,7 +2404,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -2464,7 +2470,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -2507,7 +2513,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -2537,11 +2543,14 @@
       <c r="F87" t="s">
         <v>152</v>
       </c>
+      <c r="J87" t="s">
+        <v>116</v>
+      </c>
       <c r="K87" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -2551,11 +2560,14 @@
       <c r="F88" t="s">
         <v>152</v>
       </c>
+      <c r="J88" t="s">
+        <v>116</v>
+      </c>
       <c r="K88" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -2568,11 +2580,14 @@
       <c r="G89" t="s">
         <v>116</v>
       </c>
+      <c r="J89" t="s">
+        <v>116</v>
+      </c>
       <c r="K89" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -2585,11 +2600,14 @@
       <c r="G90" t="s">
         <v>116</v>
       </c>
+      <c r="J90" t="s">
+        <v>116</v>
+      </c>
       <c r="K90" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -2599,11 +2617,14 @@
       <c r="F91" t="s">
         <v>152</v>
       </c>
+      <c r="J91" t="s">
+        <v>116</v>
+      </c>
       <c r="K91" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -2613,6 +2634,9 @@
       <c r="F92" t="s">
         <v>153</v>
       </c>
+      <c r="J92" t="s">
+        <v>116</v>
+      </c>
       <c r="K92" t="s">
         <v>154</v>
       </c>
@@ -2620,7 +2644,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -2630,6 +2654,9 @@
       <c r="F93" t="s">
         <v>153</v>
       </c>
+      <c r="J93" t="s">
+        <v>116</v>
+      </c>
       <c r="K93" t="s">
         <v>154</v>
       </c>
@@ -2637,7 +2664,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -2647,11 +2674,14 @@
       <c r="F94" t="s">
         <v>152</v>
       </c>
+      <c r="J94" t="s">
+        <v>116</v>
+      </c>
       <c r="K94" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -2661,11 +2691,14 @@
       <c r="F95" t="s">
         <v>152</v>
       </c>
+      <c r="J95" t="s">
+        <v>116</v>
+      </c>
       <c r="K95" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -2675,6 +2708,9 @@
       <c r="F96" t="s">
         <v>153</v>
       </c>
+      <c r="J96" t="s">
+        <v>116</v>
+      </c>
       <c r="K96" t="s">
         <v>154</v>
       </c>
@@ -2682,7 +2718,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -2692,6 +2728,9 @@
       <c r="F97" t="s">
         <v>153</v>
       </c>
+      <c r="J97" t="s">
+        <v>116</v>
+      </c>
       <c r="K97" t="s">
         <v>154</v>
       </c>
@@ -2699,7 +2738,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -2709,6 +2748,9 @@
       <c r="F98" t="s">
         <v>153</v>
       </c>
+      <c r="J98" t="s">
+        <v>116</v>
+      </c>
       <c r="K98" t="s">
         <v>154</v>
       </c>
@@ -2716,7 +2758,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -2726,11 +2768,14 @@
       <c r="F99" t="s">
         <v>152</v>
       </c>
+      <c r="J99" t="s">
+        <v>116</v>
+      </c>
       <c r="K99" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -2740,11 +2785,14 @@
       <c r="F100" t="s">
         <v>152</v>
       </c>
+      <c r="J100" t="s">
+        <v>116</v>
+      </c>
       <c r="K100" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -2757,8 +2805,11 @@
       <c r="F101" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J101" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -2778,7 +2829,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -2795,7 +2846,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -2812,7 +2863,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -2829,7 +2880,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -2837,11 +2888,11 @@
         <v>107</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" ref="F98:F110" si="0">IF(L106&gt;0,"Y","")</f>
+        <f t="shared" ref="F106:F110" si="0">IF(L106&gt;0,"Y","")</f>
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>112</v>
       </c>
@@ -2853,7 +2904,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>112</v>
       </c>
@@ -2865,7 +2916,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>112</v>
       </c>
@@ -2877,7 +2928,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -2969,50 +3020,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6087F05D-D7E6-4043-85A1-63840D765DFB}">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:I36"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1214</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -3020,7 +3075,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1221</v>
       </c>
@@ -3028,7 +3083,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -3036,7 +3091,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1239</v>
       </c>
@@ -3044,17 +3099,17 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>742</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>100</v>
       </c>
@@ -3062,7 +3117,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>838</v>
       </c>
@@ -3070,7 +3125,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -3078,7 +3133,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1345</v>
       </c>
@@ -3086,54 +3141,54 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
     </row>
   </sheetData>
@@ -3151,17 +3206,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.88671875" customWidth="1"/>
-    <col min="3" max="3" width="39.5546875" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>128</v>
       </c>
@@ -3178,7 +3233,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3192,7 +3247,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -3206,7 +3261,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -3223,7 +3278,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -3237,7 +3292,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>

</xml_diff>